<commit_message>
Mise en place fonction qui retourne les infos sur le port série Signed-off-by: Sebastien <mrtseb14@gmail.com>
</commit_message>
<xml_diff>
--- a/CeC - API Véhicule - V1.9.xlsx
+++ b/CeC - API Véhicule - V1.9.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\COURSE EN COURS\PRIT006403 - Véhicule v1.0\1- CDC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_cours\2nde\CITEC\CeC\_cec 2019\CeC AC Caen 23-01-2020\cec-arduino\CeC_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BC53CB-5051-4A97-9F7B-1EBFD8F2BB2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23381B74-B421-49CC-9902-3252EDA7CA96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="831" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2490" yWindow="2130" windowWidth="8700" windowHeight="11385" tabRatio="831" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="13" r:id="rId1"/>
@@ -3436,7 +3436,7 @@
   </sheetPr>
   <dimension ref="D11:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
@@ -4685,7 +4685,7 @@
   <dimension ref="B3:L42"/>
   <sheetViews>
     <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5106,7 +5106,7 @@
   </sheetPr>
   <dimension ref="C3:V21"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Y39" sqref="Y39"/>
     </sheetView>
   </sheetViews>
@@ -5366,7 +5366,7 @@
   <dimension ref="C3:D28"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5448,7 +5448,7 @@
   </sheetPr>
   <dimension ref="B3:H45"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B7" workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
@@ -5849,7 +5849,7 @@
   <dimension ref="C5:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6286,8 +6286,8 @@
   </sheetPr>
   <dimension ref="B3:H38"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10268,18 +10268,18 @@
     <row r="96" spans="3:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C78:C93"/>
+    <mergeCell ref="C53:H53"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="C56:C71"/>
+    <mergeCell ref="C75:H75"/>
+    <mergeCell ref="C76:C77"/>
     <mergeCell ref="C33:C48"/>
     <mergeCell ref="C8:H8"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="C11:C26"/>
     <mergeCell ref="C30:H30"/>
     <mergeCell ref="C31:C32"/>
-    <mergeCell ref="C78:C93"/>
-    <mergeCell ref="C53:H53"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="C56:C71"/>
-    <mergeCell ref="C75:H75"/>
-    <mergeCell ref="C76:C77"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>